<commit_message>
web solo detecta uno
</commit_message>
<xml_diff>
--- a/web/data/nombre3.xlsx
+++ b/web/data/nombre3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Pictures\Screenshots\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Mogro\Certificados dinámicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7008A9-58F4-42D0-8A0D-358524818F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E3B036-4AA4-4B37-B12E-7E0D617D0A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -424,7 +424,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>